<commit_message>
correction: fix Program 2
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 2.xlsx
+++ b/Convert to Binary_v3 - Program 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Program2.txt" sheetId="1" r:id="rId1"/>
@@ -1171,7 +1171,7 @@
     <t>LDR 2,2,1,23(i)</t>
   </si>
   <si>
-    <t>AIR 0,22</t>
+    <t>AIR 0,28</t>
   </si>
 </sst>
 </file>
@@ -1675,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -3420,7 +3420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="J15" s="9" t="str">
         <f t="shared" si="16"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K15" s="9">
         <f t="shared" si="17"/>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="T15" s="17" t="str">
         <f t="shared" si="21"/>
-        <v>10110</v>
+        <v>11100</v>
       </c>
       <c r="U15" s="17" t="str">
         <f t="shared" si="22"/>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="Y15" s="10" t="str">
         <f t="shared" si="26"/>
-        <v>00010110</v>
+        <v>00011100</v>
       </c>
       <c r="Z15" s="10" t="str">
         <f t="shared" si="27"/>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="AB15" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0001100000010110</v>
+        <v>0001100000011100</v>
       </c>
       <c r="AC15" s="10">
         <f t="shared" si="30"/>

</xml_diff>

<commit_message>
Program 2 finally works
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 2.xlsx
+++ b/Convert to Binary_v3 - Program 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Program2.txt" sheetId="1" r:id="rId1"/>
@@ -553,9 +553,6 @@
     <t>Unconditional jump to SEARCH WORD INPUT LOOP START</t>
   </si>
   <si>
-    <t>Store the Enter character (R3) into the Search Word Character Address; SEARCH WORD INPUT LOOP END</t>
-  </si>
-  <si>
     <t>Reset contents of File Input Character Address to the start of the array (stored in a)</t>
   </si>
   <si>
@@ -751,9 +748,6 @@
     <t>Unconditional jump to PRINT SEARCH WORD LOOP START</t>
   </si>
   <si>
-    <t>OUT 0,2</t>
-  </si>
-  <si>
     <t>Output sentence number of search word (1-6, stored in R0)--NOT ASCII</t>
   </si>
   <si>
@@ -772,15 +766,9 @@
     <t>If the quotient (in R2) = 0, jump to PRINT ONES DIGIT</t>
   </si>
   <si>
-    <t>OUT 2,2</t>
-  </si>
-  <si>
     <t>Else, output the tens digit (R2)--NOT ASCII</t>
   </si>
   <si>
-    <t>OUT 3,2</t>
-  </si>
-  <si>
     <t>Output the remainder/ones digit (in R3)--NOT ASCII; PRINT ONES DIGIT</t>
   </si>
   <si>
@@ -1138,9 +1126,6 @@
     <t>SRC 3,0,1,3</t>
   </si>
   <si>
-    <t>SRC 3,0,1,2</t>
-  </si>
-  <si>
     <t>AIR 3,14</t>
   </si>
   <si>
@@ -1169,6 +1154,21 @@
   </si>
   <si>
     <t>LDR 2,3,1,23(i)</t>
+  </si>
+  <si>
+    <t>STR 3,3,1,25(x)</t>
+  </si>
+  <si>
+    <t>Store the Enter character (R3) into address indirect addressed by the Search Word Character Address; SEARCH WORD INPUT LOOP END</t>
+  </si>
+  <si>
+    <t>OUT 0,1</t>
+  </si>
+  <si>
+    <t>OUT 2,1</t>
+  </si>
+  <si>
+    <t>OUT 3,1</t>
   </si>
 </sst>
 </file>
@@ -1672,31 +1672,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView topLeftCell="A218" workbookViewId="0">
+      <selection sqref="A1:A247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1714,18 +1714,18 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1740,18 +1740,18 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,44 +1766,44 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E14" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E17" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D19" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,12 +1811,12 @@
         <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1824,12 +1824,12 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1866,20 +1866,20 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D28" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1889,10 +1889,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F32" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,10 +1902,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F34" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1915,10 +1915,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F36" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1928,7 +1928,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D38" t="s">
         <v>148</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1946,15 +1946,15 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E41" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1964,10 +1964,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F44" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1977,10 +1977,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F46" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,10 +1990,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>323</v>
+      </c>
+      <c r="F48" t="s">
         <v>327</v>
-      </c>
-      <c r="F48" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2003,10 +2003,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F50" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2016,10 +2016,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E52" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2058,7 +2058,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C58" t="s">
         <v>154</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D59" t="s">
         <v>155</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D61" t="s">
         <v>157</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D63" t="s">
         <v>160</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D64" t="s">
         <v>161</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D65" t="s">
         <v>162</v>
@@ -2143,15 +2143,15 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E69" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2161,10 +2161,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F72" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2174,10 +2174,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F74" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,10 +2187,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E76" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2208,7 +2208,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2218,15 +2218,15 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E81" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2236,10 +2236,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F84" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2249,10 +2249,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F86" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2262,10 +2262,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E88" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -2283,7 +2283,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2293,15 +2293,15 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E93" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2311,10 +2311,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F96" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -2332,7 +2332,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2342,15 +2342,15 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E101" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2360,10 +2360,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F104" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2373,10 +2373,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F106" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2386,10 +2386,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E108" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2428,7 +2428,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F114" t="s">
         <v>167</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C116" t="s">
         <v>169</v>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D117" t="s">
         <v>170</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D118" t="s">
         <v>171</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D120" t="s">
         <v>172</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C121" t="s">
         <v>173</v>
@@ -2492,60 +2492,60 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>274</v>
+        <v>375</v>
       </c>
       <c r="D122" t="s">
-        <v>174</v>
+        <v>376</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D123" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D125" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E127" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>176</v>
+      </c>
+      <c r="D128" t="s">
         <v>177</v>
-      </c>
-      <c r="D128" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E129" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -2553,7 +2553,7 @@
         <v>136</v>
       </c>
       <c r="D130" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -2561,15 +2561,15 @@
         <v>0</v>
       </c>
       <c r="E131" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E132" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -2587,7 +2587,7 @@
         <v>2</v>
       </c>
       <c r="E135" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -2595,7 +2595,7 @@
         <v>140</v>
       </c>
       <c r="E136" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -2603,39 +2603,39 @@
         <v>10</v>
       </c>
       <c r="E137" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D138" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>183</v>
+      </c>
+      <c r="D139" t="s">
         <v>184</v>
-      </c>
-      <c r="D139" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>185</v>
+      </c>
+      <c r="F140" t="s">
         <v>186</v>
-      </c>
-      <c r="F140" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C141" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -2643,47 +2643,47 @@
         <v>143</v>
       </c>
       <c r="E142" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D143" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C144" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>191</v>
+      </c>
+      <c r="E145" t="s">
         <v>192</v>
-      </c>
-      <c r="E145" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C146" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C147" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,7 +2691,7 @@
         <v>145</v>
       </c>
       <c r="D148" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -2699,23 +2699,23 @@
         <v>152</v>
       </c>
       <c r="F149" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C150" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F151" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -2723,23 +2723,23 @@
         <v>152</v>
       </c>
       <c r="F152" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C153" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="E154" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -2747,55 +2747,55 @@
         <v>152</v>
       </c>
       <c r="F155" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C156" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D157" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D158" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C159" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D161" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -2803,20 +2803,20 @@
         <v>158</v>
       </c>
       <c r="F162" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D163" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -2824,55 +2824,55 @@
         <v>5</v>
       </c>
       <c r="E165" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D166" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>213</v>
+      </c>
+      <c r="E167" t="s">
         <v>214</v>
-      </c>
-      <c r="E167" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C169" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D170" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D171" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -2880,7 +2880,7 @@
         <v>139</v>
       </c>
       <c r="F172" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -2888,23 +2888,23 @@
         <v>12</v>
       </c>
       <c r="E173" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C174" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D175" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -2912,15 +2912,15 @@
         <v>152</v>
       </c>
       <c r="F176" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C177" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -2928,28 +2928,28 @@
         <v>5</v>
       </c>
       <c r="E178" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C180" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D181" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -2957,36 +2957,36 @@
         <v>6</v>
       </c>
       <c r="F182" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D183" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E184" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D186" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -2994,44 +2994,44 @@
         <v>6</v>
       </c>
       <c r="F187" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D188" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D189" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D190" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D192" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
@@ -3039,7 +3039,7 @@
         <v>165</v>
       </c>
       <c r="D193" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -3047,15 +3047,15 @@
         <v>152</v>
       </c>
       <c r="F194" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C195" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -3063,15 +3063,15 @@
         <v>147</v>
       </c>
       <c r="F196" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D197" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -3084,18 +3084,18 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D199" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C200" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
@@ -3103,7 +3103,7 @@
         <v>163</v>
       </c>
       <c r="D201" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
@@ -3113,15 +3113,15 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E203" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
@@ -3131,10 +3131,10 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E206" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
@@ -3144,10 +3144,10 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F208" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -3157,10 +3157,10 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F210" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
@@ -3170,10 +3170,10 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E212" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
@@ -3183,10 +3183,10 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F214" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
@@ -3196,10 +3196,10 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E216" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
@@ -3209,10 +3209,10 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F218" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
@@ -3230,7 +3230,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,18 +3240,18 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>240</v>
+        <v>377</v>
       </c>
       <c r="F223" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E224" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -3261,7 +3261,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E226" t="s">
         <v>148</v>
@@ -3274,15 +3274,15 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E228" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,10 +3292,10 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F231" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -3305,10 +3305,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F233" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
@@ -3318,10 +3318,10 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E235" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -3339,7 +3339,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -3349,15 +3349,15 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D240" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -3365,7 +3365,7 @@
         <v>9</v>
       </c>
       <c r="D242" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -3373,31 +3373,31 @@
         <v>11</v>
       </c>
       <c r="F243" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D244" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>247</v>
-      </c>
-      <c r="F245" t="s">
-        <v>248</v>
+        <v>378</v>
+      </c>
+      <c r="E245" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>249</v>
-      </c>
-      <c r="F246" t="s">
-        <v>250</v>
+        <v>379</v>
+      </c>
+      <c r="E246" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -3405,7 +3405,7 @@
         <v>13</v>
       </c>
       <c r="G247" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3417,11 +3417,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P121" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A149" sqref="A149"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3448,7 +3448,7 @@
         <v>125</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>16</v>
@@ -3460,7 +3460,7 @@
         <v>18</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>19</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B2" s="9" t="str">
         <f t="shared" ref="B2" si="0">LEFT(A2,3)</f>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B3" s="9" t="str">
         <f t="shared" ref="B3:B66" si="8">LEFT(A3,3)</f>
@@ -3763,7 +3763,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B4" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4114,7 +4114,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B7" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4582,7 +4582,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B11" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4699,7 +4699,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5050,7 +5050,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B15" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5167,7 +5167,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B16" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5284,7 +5284,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B17" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5401,7 +5401,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5518,7 +5518,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B19" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5635,7 +5635,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6103,7 +6103,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B24" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6688,7 +6688,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B29" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6805,7 +6805,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B30" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6922,7 +6922,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B31" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7156,7 +7156,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B33" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7390,7 +7390,7 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B35" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7624,7 +7624,7 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B37" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7858,7 +7858,7 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B39" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7975,7 +7975,7 @@
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B40" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8209,7 +8209,7 @@
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B42" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8326,7 +8326,7 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B43" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8560,7 +8560,7 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B45" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8794,7 +8794,7 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B47" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9028,7 +9028,7 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B49" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9262,7 +9262,7 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B51" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9496,7 +9496,7 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B53" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10198,7 +10198,7 @@
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B59" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10315,7 +10315,7 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B60" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10549,7 +10549,7 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B62" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10783,7 +10783,7 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B64" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10900,7 +10900,7 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B65" s="9" t="str">
         <f t="shared" si="8"/>
@@ -11017,7 +11017,7 @@
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B66" s="9" t="str">
         <f t="shared" si="8"/>
@@ -11485,7 +11485,7 @@
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B70" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11602,7 +11602,7 @@
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B71" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11836,7 +11836,7 @@
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B73" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12070,7 +12070,7 @@
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B75" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12304,7 +12304,7 @@
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B77" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12655,7 +12655,7 @@
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B80" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12889,7 +12889,7 @@
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B82" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13006,7 +13006,7 @@
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B83" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13240,7 +13240,7 @@
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B85" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13474,7 +13474,7 @@
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B87" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13708,7 +13708,7 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B89" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14059,7 +14059,7 @@
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B92" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14293,7 +14293,7 @@
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B94" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14410,7 +14410,7 @@
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B95" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14644,7 +14644,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14995,7 +14995,7 @@
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B100" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15229,7 +15229,7 @@
     </row>
     <row r="102" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B102" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15346,7 +15346,7 @@
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B103" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15580,7 +15580,7 @@
     </row>
     <row r="105" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B105" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15814,7 +15814,7 @@
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B107" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16048,7 +16048,7 @@
     </row>
     <row r="109" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B109" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16750,7 +16750,7 @@
     </row>
     <row r="115" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B115" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16984,7 +16984,7 @@
     </row>
     <row r="117" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A117" s="12" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B117" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17101,7 +17101,7 @@
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B118" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17218,7 +17218,7 @@
     </row>
     <row r="119" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B119" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17452,7 +17452,7 @@
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B121" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17569,7 +17569,7 @@
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A122" s="12" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B122" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17686,7 +17686,7 @@
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" s="12" t="s">
-        <v>274</v>
+        <v>375</v>
       </c>
       <c r="B123" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17726,7 +17726,7 @@
       </c>
       <c r="K123" s="9" t="str">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L123" s="9" t="str">
         <f t="shared" si="41"/>
@@ -17766,7 +17766,7 @@
       </c>
       <c r="U123" s="17" t="str">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V123" s="17" t="str">
         <f t="shared" si="46"/>
@@ -17786,7 +17786,7 @@
       </c>
       <c r="Z123" s="10" t="str">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA123" s="10" t="str">
         <f t="shared" si="51"/>
@@ -17794,7 +17794,7 @@
       </c>
       <c r="AB123" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0000101111011001</v>
+        <v>0000101111111001</v>
       </c>
       <c r="AC123" s="10">
         <f t="shared" si="53"/>
@@ -17803,7 +17803,7 @@
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A124" s="12" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B124" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17920,7 +17920,7 @@
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B125" s="9" t="str">
         <f t="shared" si="31"/>
@@ -18037,7 +18037,7 @@
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A126" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B126" s="9" t="str">
         <f t="shared" si="31"/>
@@ -18154,7 +18154,7 @@
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B127" s="9" t="str">
         <f t="shared" si="31"/>
@@ -18271,7 +18271,7 @@
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B128" s="9" t="str">
         <f t="shared" si="31"/>
@@ -18388,7 +18388,7 @@
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B129" s="9" t="str">
         <f t="shared" si="31"/>
@@ -18505,7 +18505,7 @@
     </row>
     <row r="130" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A130" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B130" s="9" t="str">
         <f t="shared" si="31"/>
@@ -18856,7 +18856,7 @@
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B133" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19558,7 +19558,7 @@
     </row>
     <row r="139" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A139" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B139" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19675,7 +19675,7 @@
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A140" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B140" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19792,7 +19792,7 @@
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B141" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19909,7 +19909,7 @@
     </row>
     <row r="142" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A142" s="12" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B142" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20143,7 +20143,7 @@
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B144" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20260,7 +20260,7 @@
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B145" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20377,7 +20377,7 @@
     </row>
     <row r="146" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A146" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B146" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20494,7 +20494,7 @@
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A147" s="12" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B147" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20611,7 +20611,7 @@
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B148" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20962,7 +20962,7 @@
     </row>
     <row r="151" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A151" s="12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B151" s="9" t="str">
         <f t="shared" si="54"/>
@@ -21079,7 +21079,7 @@
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B152" s="9" t="str">
         <f t="shared" si="54"/>
@@ -21313,7 +21313,7 @@
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A154" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B154" s="9" t="str">
         <f t="shared" si="54"/>
@@ -21430,7 +21430,7 @@
     </row>
     <row r="155" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A155" s="12" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B155" s="9" t="str">
         <f t="shared" si="54"/>
@@ -21664,7 +21664,7 @@
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A157" s="12" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B157" s="9" t="str">
         <f t="shared" si="54"/>
@@ -21781,7 +21781,7 @@
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A158" s="12" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B158" s="9" t="str">
         <f t="shared" si="54"/>
@@ -21898,7 +21898,7 @@
     </row>
     <row r="159" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A159" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B159" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22015,7 +22015,7 @@
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A160" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B160" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22132,7 +22132,7 @@
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A161" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B161" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22249,7 +22249,7 @@
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A162" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B162" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22483,7 +22483,7 @@
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A164" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B164" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22600,7 +22600,7 @@
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A165" s="12" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B165" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22834,7 +22834,7 @@
     </row>
     <row r="167" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A167" s="12" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B167" s="9" t="str">
         <f t="shared" si="54"/>
@@ -22951,7 +22951,7 @@
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A168" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B168" s="9" t="str">
         <f t="shared" si="54"/>
@@ -23068,7 +23068,7 @@
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A169" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B169" s="9" t="str">
         <f t="shared" si="54"/>
@@ -23185,7 +23185,7 @@
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A170" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B170" s="9" t="str">
         <f t="shared" si="54"/>
@@ -23302,7 +23302,7 @@
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A171" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B171" s="9" t="str">
         <f t="shared" si="54"/>
@@ -23419,7 +23419,7 @@
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B172" s="9" t="str">
         <f t="shared" si="54"/>
@@ -23770,7 +23770,7 @@
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B175" s="9" t="str">
         <f t="shared" si="54"/>
@@ -23887,7 +23887,7 @@
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B176" s="9" t="str">
         <f t="shared" si="54"/>
@@ -24121,7 +24121,7 @@
     </row>
     <row r="178" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B178" s="9" t="str">
         <f t="shared" si="54"/>
@@ -24355,7 +24355,7 @@
     </row>
     <row r="180" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A180" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B180" s="9" t="str">
         <f t="shared" si="54"/>
@@ -24472,7 +24472,7 @@
     </row>
     <row r="181" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A181" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B181" s="9" t="str">
         <f t="shared" si="54"/>
@@ -24589,7 +24589,7 @@
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A182" s="12" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B182" s="9" t="str">
         <f t="shared" si="54"/>
@@ -24823,7 +24823,7 @@
     </row>
     <row r="184" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A184" s="12" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B184" s="9" t="str">
         <f t="shared" si="54"/>
@@ -24940,7 +24940,7 @@
     </row>
     <row r="185" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B185" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25057,7 +25057,7 @@
     </row>
     <row r="186" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A186" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B186" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25174,7 +25174,7 @@
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A187" s="12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B187" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25408,7 +25408,7 @@
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A189" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B189" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25525,7 +25525,7 @@
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A190" s="12" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B190" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25642,7 +25642,7 @@
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A191" s="12" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B191" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25759,7 +25759,7 @@
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B192" s="9" t="str">
         <f t="shared" si="54"/>
@@ -25876,7 +25876,7 @@
     </row>
     <row r="193" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B193" s="9" t="str">
         <f t="shared" si="54"/>
@@ -26227,7 +26227,7 @@
     </row>
     <row r="196" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B196" s="9" t="str">
         <f t="shared" si="77"/>
@@ -26461,7 +26461,7 @@
     </row>
     <row r="198" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B198" s="9" t="str">
         <f t="shared" si="77"/>
@@ -26695,7 +26695,7 @@
     </row>
     <row r="200" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B200" s="9" t="str">
         <f t="shared" si="77"/>
@@ -26812,7 +26812,7 @@
     </row>
     <row r="201" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B201" s="9" t="str">
         <f t="shared" si="77"/>
@@ -27163,7 +27163,7 @@
     </row>
     <row r="204" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A204" s="12" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B204" s="9" t="str">
         <f t="shared" si="77"/>
@@ -27280,7 +27280,7 @@
     </row>
     <row r="205" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A205" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B205" s="9" t="str">
         <f t="shared" si="77"/>
@@ -27514,7 +27514,7 @@
     </row>
     <row r="207" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A207" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B207" s="9" t="str">
         <f t="shared" si="77"/>
@@ -27748,7 +27748,7 @@
     </row>
     <row r="209" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A209" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B209" s="9" t="str">
         <f t="shared" si="77"/>
@@ -27982,7 +27982,7 @@
     </row>
     <row r="211" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A211" s="12" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B211" s="9" t="str">
         <f t="shared" si="77"/>
@@ -28216,7 +28216,7 @@
     </row>
     <row r="213" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A213" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B213" s="9" t="str">
         <f t="shared" si="77"/>
@@ -28450,7 +28450,7 @@
     </row>
     <row r="215" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A215" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B215" s="9" t="str">
         <f t="shared" si="77"/>
@@ -28684,7 +28684,7 @@
     </row>
     <row r="217" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A217" s="12" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B217" s="9" t="str">
         <f t="shared" si="77"/>
@@ -28918,7 +28918,7 @@
     </row>
     <row r="219" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A219" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B219" s="9" t="str">
         <f t="shared" si="77"/>
@@ -29269,7 +29269,7 @@
     </row>
     <row r="222" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B222" s="9" t="str">
         <f t="shared" si="77"/>
@@ -29503,7 +29503,7 @@
     </row>
     <row r="224" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A224" s="12" t="s">
-        <v>240</v>
+        <v>377</v>
       </c>
       <c r="B224" s="9" t="str">
         <f t="shared" si="77"/>
@@ -29539,7 +29539,7 @@
       </c>
       <c r="J224" s="9" t="str">
         <f t="shared" si="85"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K224" s="9">
         <f t="shared" si="86"/>
@@ -29579,7 +29579,7 @@
       </c>
       <c r="T224" s="17" t="str">
         <f t="shared" si="90"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="U224" s="17" t="str">
         <f t="shared" si="91"/>
@@ -29599,7 +29599,7 @@
       </c>
       <c r="Y224" s="10" t="str">
         <f t="shared" si="95"/>
-        <v>00000010</v>
+        <v>00000001</v>
       </c>
       <c r="Z224" s="10" t="str">
         <f t="shared" si="96"/>
@@ -29611,7 +29611,7 @@
       </c>
       <c r="AB224" s="11" t="str">
         <f t="shared" si="98"/>
-        <v>1100100000000010</v>
+        <v>1100100000000001</v>
       </c>
       <c r="AC224" s="10">
         <f t="shared" si="99"/>
@@ -29620,7 +29620,7 @@
     </row>
     <row r="225" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A225" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B225" s="9" t="str">
         <f t="shared" si="77"/>
@@ -29854,7 +29854,7 @@
     </row>
     <row r="227" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A227" s="12" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B227" s="9" t="str">
         <f t="shared" si="77"/>
@@ -30088,7 +30088,7 @@
     </row>
     <row r="229" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A229" s="12" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B229" s="9" t="str">
         <f t="shared" si="77"/>
@@ -30132,7 +30132,7 @@
       </c>
       <c r="L229" s="9" t="str">
         <f t="shared" si="87"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M229" s="22" t="str">
         <f>VLOOKUP($B229,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -30172,7 +30172,7 @@
       </c>
       <c r="V229" s="17" t="str">
         <f t="shared" si="92"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="W229" s="15" t="str">
         <f t="shared" si="93"/>
@@ -30192,11 +30192,11 @@
       </c>
       <c r="AA229" s="10" t="str">
         <f t="shared" si="97"/>
-        <v>000010</v>
+        <v>000001</v>
       </c>
       <c r="AB229" s="11" t="str">
         <f t="shared" si="98"/>
-        <v>0110011101000010</v>
+        <v>0110011101000001</v>
       </c>
       <c r="AC229" s="10">
         <f t="shared" si="99"/>
@@ -30205,7 +30205,7 @@
     </row>
     <row r="230" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B230" s="9" t="str">
         <f t="shared" si="77"/>
@@ -30439,7 +30439,7 @@
     </row>
     <row r="232" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A232" s="12" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B232" s="9" t="str">
         <f t="shared" si="100"/>
@@ -30673,7 +30673,7 @@
     </row>
     <row r="234" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A234" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B234" s="9" t="str">
         <f t="shared" si="100"/>
@@ -30907,7 +30907,7 @@
     </row>
     <row r="236" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A236" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B236" s="9" t="str">
         <f t="shared" ref="B236:B248" si="114">LEFT(A236,3)</f>
@@ -31258,7 +31258,7 @@
     </row>
     <row r="239" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A239" s="12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B239" s="9" t="str">
         <f t="shared" si="114"/>
@@ -31492,7 +31492,7 @@
     </row>
     <row r="241" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A241" s="12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B241" s="9" t="str">
         <f t="shared" si="114"/>
@@ -31609,7 +31609,7 @@
     </row>
     <row r="242" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A242" s="12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B242" s="9" t="str">
         <f t="shared" si="114"/>
@@ -31960,7 +31960,7 @@
     </row>
     <row r="245" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A245" s="12" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B245" s="9" t="str">
         <f t="shared" si="114"/>
@@ -32077,7 +32077,7 @@
     </row>
     <row r="246" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A246" s="12" t="s">
-        <v>247</v>
+        <v>378</v>
       </c>
       <c r="B246" s="9" t="str">
         <f t="shared" si="114"/>
@@ -32113,7 +32113,7 @@
       </c>
       <c r="J246" s="9" t="str">
         <f t="shared" si="85"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K246" s="9">
         <f t="shared" si="86"/>
@@ -32153,7 +32153,7 @@
       </c>
       <c r="T246" s="17" t="str">
         <f t="shared" si="118"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="U246" s="17" t="str">
         <f t="shared" si="119"/>
@@ -32173,7 +32173,7 @@
       </c>
       <c r="Y246" s="10" t="str">
         <f t="shared" si="123"/>
-        <v>00000010</v>
+        <v>00000001</v>
       </c>
       <c r="Z246" s="10" t="str">
         <f t="shared" si="124"/>
@@ -32185,7 +32185,7 @@
       </c>
       <c r="AB246" s="11" t="str">
         <f t="shared" si="126"/>
-        <v>1100101000000010</v>
+        <v>1100101000000001</v>
       </c>
       <c r="AC246" s="10">
         <f t="shared" si="127"/>
@@ -32194,7 +32194,7 @@
     </row>
     <row r="247" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A247" s="12" t="s">
-        <v>249</v>
+        <v>379</v>
       </c>
       <c r="B247" s="9" t="str">
         <f t="shared" si="114"/>
@@ -32230,7 +32230,7 @@
       </c>
       <c r="J247" s="9" t="str">
         <f t="shared" si="85"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K247" s="9">
         <f t="shared" si="86"/>
@@ -32270,7 +32270,7 @@
       </c>
       <c r="T247" s="17" t="str">
         <f t="shared" si="118"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="U247" s="17" t="str">
         <f t="shared" si="119"/>
@@ -32290,7 +32290,7 @@
       </c>
       <c r="Y247" s="10" t="str">
         <f t="shared" si="123"/>
-        <v>00000010</v>
+        <v>00000001</v>
       </c>
       <c r="Z247" s="10" t="str">
         <f t="shared" si="124"/>
@@ -32302,7 +32302,7 @@
       </c>
       <c r="AB247" s="11" t="str">
         <f t="shared" si="126"/>
-        <v>1100101100000010</v>
+        <v>1100101100000001</v>
       </c>
       <c r="AC247" s="10">
         <f t="shared" si="127"/>

</xml_diff>